<commit_message>
fix bugs and add toefl mode
</commit_message>
<xml_diff>
--- a/public/format_blast.xlsx
+++ b/public/format_blast.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Project\blast-whatsapp\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miftahul.arifin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>No</t>
   </si>
@@ -41,10 +41,22 @@
     <t>Miftahul Arifin</t>
   </si>
   <si>
+    <t>081286203011</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Listening</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>Arifin</t>
-  </si>
-  <si>
-    <t>081286203011</t>
   </si>
 </sst>
 </file>
@@ -366,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -380,7 +392,7 @@
     <col min="4" max="4" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -393,8 +405,20 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -402,16 +426,28 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D4" s="1"/>
     </row>
   </sheetData>

</xml_diff>